<commit_message>
v2 添加: lua, json导出支持
</commit_message>
<xml_diff>
--- a/exportorv2/test/Sample.xlsx
+++ b/exportorv2/test/Sample.xlsx
@@ -432,10 +432,6 @@
   </si>
   <si>
     <t>int64</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>RepeatCheck:true</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -638,6 +634,10 @@
   </si>
   <si>
     <t>物品id</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RepeatCheck:true LuaIndex:true</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -1129,28 +1129,28 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
@@ -1164,43 +1164,43 @@
         <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -1214,13 +1214,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>
@@ -1250,13 +1250,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
@@ -1354,41 +1354,41 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1396,58 +1396,58 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>